<commit_message>
[MDTUDDM-25757] Registry operational zone
Change-Id: Ib466f5f1229da54d1f6c5ae15681ded2ee115ebf
</commit_message>
<xml_diff>
--- a/docs/ua/modules/arch/attachments/architecture/registry_cost_calculator.xlsx
+++ b/docs/ua/modules/arch/attachments/architecture/registry_cost_calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/modules/arch/attachments/architecture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Maksym_Kharchenko/Work/Development/mdtu-ddm/mdtu-ddm-gerrit-workspace/mdtu-ddm/general/ddm-architecture/docs/ua/modules/arch/attachments/architecture/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48401AEA-D67E-EF40-AAF6-7E47D034297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF37101B-D7D8-8F4B-AB73-DAB13B4B6AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{27F18D04-7E62-4946-83A8-E11013D50C84}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{27F18D04-7E62-4946-83A8-E11013D50C84}"/>
   </bookViews>
   <sheets>
     <sheet name="Калькулятор вартості" sheetId="1" r:id="rId1"/>
@@ -1733,7 +1733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A819B9D-8FE0-401F-8C51-9F6F8ACD5799}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -2225,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C2CE02-549B-42BB-BB2B-79BD8E0A657F}">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2260,7 +2260,7 @@
         <v>76</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>77</v>
@@ -2870,6 +2870,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010022314AB35D24274D94E93A0CCD2DBC5F" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3febe1d67782b5c77e50c43cf0e433a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="346a80a9-3278-4844-b436-58ae57568790" xmlns:ns3="a2d094e0-efa8-4820-a0b3-29af30f3c512" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a828650ea744d4614f15fd37c541cd95" ns2:_="" ns3:_="">
     <xsd:import namespace="346a80a9-3278-4844-b436-58ae57568790"/>
@@ -3128,15 +3137,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3163,6 +3163,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FEC7CF-4815-42BA-A053-9D2F9AB7FD60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D39A1E4B-89AB-4EF2-84C8-5084CDAB4D34}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3181,14 +3189,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FEC7CF-4815-42BA-A053-9D2F9AB7FD60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD363066-8CBD-4D6F-8835-7EB8A1E12EC9}">
   <ds:schemaRefs>

</xml_diff>